<commit_message>
Add visualization scripts and configuration files for aggression analysis
</commit_message>
<xml_diff>
--- a/data/labeling.xlsx
+++ b/data/labeling.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728A911D-C9E1-4831-B0ED-E1F409037A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74C5FB5-46E7-4349-801C-AA389B2405B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>היום ההורה שלי עזר/ה לי במשהו (כמו הקפצה לחוג/תנועת נוער, עזרה בשיעורי בית וכו')</t>
   </si>
@@ -28,25 +28,16 @@
     <t>היום ההורה שלי דיבר/ה איתי על החברים שלי או על היום שלי</t>
   </si>
   <si>
-    <t>Inconsistent discipline</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, ההורה שלי איים/ה להעניש אותי אבל לא עשה/תה זאת</t>
   </si>
   <si>
     <t>מאז הסקר האחרון, ההורה שלי החמיא/ה לי כשעשיתי משהו בצורה טובה</t>
   </si>
   <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, הרגשתי מודאג/ת או מפוחד/ת.</t>
   </si>
   <si>
     <t>ברגע זה, אני מרגיש/ה פחד או לחץ</t>
-  </si>
-  <si>
-    <t>Agression</t>
   </si>
   <si>
     <t>מאז הסקר האחרון, התפרצתי בכעס באחת או יותר מהדרכים הבאות:
@@ -64,18 +55,12 @@
     <t>מאז הסקר האחרון, כעסתי או התעצבנתי כשדברים קרו לא כמו שרציתי</t>
   </si>
   <si>
-    <t>Irritability</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, הרגשתי מתוסכל/ת.</t>
   </si>
   <si>
     <t>ברגע זה, אני מרגיש/ה מרוגז/ת או כועס/ת</t>
   </si>
   <si>
-    <t>Parent-Child</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, עצבנתי את ההורה שלי</t>
   </si>
   <si>
@@ -85,46 +70,25 @@
     <t>מאז הסקר האחרון, שיתפתי את ההורה ברגשות/תחושות שלי (שאני שמח/ה, עצוב/ה, כועס/ת, עצבני/ת, שקרה לי משהו מרגש היום)</t>
   </si>
   <si>
-    <t>Depression</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, הרגשתי עצוב/ה או מדוכא/ת</t>
   </si>
   <si>
-    <t>Mood - good</t>
-  </si>
-  <si>
     <t xml:space="preserve">ברגע זה אני מרגיש/ה טוב </t>
   </si>
   <si>
-    <t>ADHD</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, דעתי הוסחה בקלות</t>
   </si>
   <si>
-    <t>Inhibitory Control</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, יצא שאמרתי את הדבר הראשון שעלה לי לראש מבלי לעצור ולחשוב</t>
   </si>
   <si>
     <t>מאז הסקר האחרון, היה לי קשה להפסיק לעשות משהו אחרי שביקשו ממני להפסיק (לדוגמה כשמורים מבקשים ממני להפסיק לדבר בכיתה או כשההורים מבקשים ממני להפסיק להיות מול המסך)</t>
   </si>
   <si>
-    <t>Authoritarian Parenting</t>
-  </si>
-  <si>
     <t xml:space="preserve">מאז הסקר האחרון, ההורה שלי התעצבנ/ה או צעק/ה עליי </t>
   </si>
   <si>
-    <t>Authoritative Parenting</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, ההורה שלי היה סבלני/ת כלפיי</t>
-  </si>
-  <si>
-    <t>Permissive Parenting</t>
   </si>
   <si>
     <t>מאז הסקר האחרון, ההורה שלי הסכימ/ה לכל מה שרציתי</t>
@@ -212,15 +176,6 @@
   </si>
   <si>
     <t xml:space="preserve">מאז הסקר האחרון, לילד/ה שלי היה קשה להפסיק לעשות משהו כאשר ביקשו ממנו/ה להפסיק </t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>Parental involvement</t>
-  </si>
-  <si>
-    <t>Positive parenting</t>
   </si>
   <si>
     <t>ברגע זה אני מרגיש/ה חסר/ת מנוחה</t>
@@ -433,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -460,7 +415,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -469,101 +424,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -715,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -723,70 +583,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1069,450 +908,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.7109375" style="15"/>
-    <col min="4" max="16384" width="18.7109375" style="15"/>
+    <col min="1" max="2" width="18.7109375" style="12"/>
+    <col min="4" max="16384" width="18.7109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>116</v>
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="189" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="189" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="B19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="F3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="B20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="189" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6" t="s">
+    <row r="26" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="F8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="189" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="F10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="F12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="F13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="F15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="F16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="F20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="F24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="18"/>
+      <c r="F26" s="15"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B27">
     <sortCondition ref="A2:A27"/>
   </sortState>
-  <mergeCells count="8">
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D9:D10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>